<commit_message>
Upload Y4_B2526_General_Surgery_scanner1759306508930_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_scanner1759306508930_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_scanner1759306508930_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\Imported_logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BC0D95-60B7-4FE5-B1CB-A1B1D816C08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4AEB2B-65A3-41D4-A19E-4CE60F90FDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scanner" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="289">
   <si>
     <t>Student ID</t>
   </si>
@@ -887,27 +887,6 @@
   </si>
   <si>
     <t>11:53:22</t>
-  </si>
-  <si>
-    <t>190314</t>
-  </si>
-  <si>
-    <t>general surgery</t>
-  </si>
-  <si>
-    <t>14/09/2025</t>
-  </si>
-  <si>
-    <t>10:30:00</t>
-  </si>
-  <si>
-    <t>Appeal</t>
-  </si>
-  <si>
-    <t>201197</t>
-  </si>
-  <si>
-    <t>13/09/2025</t>
   </si>
 </sst>
 </file>
@@ -1285,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F143"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141:E143"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4096,57 +4075,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
-        <v>289</v>
-      </c>
-      <c r="B141" t="s">
-        <v>290</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D141" t="s">
-        <v>292</v>
-      </c>
-      <c r="E141" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
-        <v>294</v>
-      </c>
-      <c r="B142" t="s">
-        <v>290</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D142" t="s">
-        <v>292</v>
-      </c>
-      <c r="E142" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
-        <v>294</v>
-      </c>
-      <c r="B143" t="s">
-        <v>290</v>
-      </c>
-      <c r="C143" s="1">
-        <v>45914</v>
-      </c>
-      <c r="D143" t="s">
-        <v>292</v>
-      </c>
-      <c r="E143" t="s">
-        <v>293</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>